<commit_message>
feat: update forecast data and add new production verification files
</commit_message>
<xml_diff>
--- a/Procurement/EXSIM_Mezquite_Purchasing_CORREGIDO_FIX_with_policies.xlsx
+++ b/Procurement/EXSIM_Mezquite_Purchasing_CORREGIDO_FIX_with_policies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc407a335d7300f/Documentos/GitHub/BusinessSim/Procurement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1809" documentId="6_{4F45DE64-BE33-4F18-9BCE-C4F36FED717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7643515E-B572-4153-B2B3-0A9CBFFA41B0}"/>
+  <xr:revisionPtr revIDLastSave="2149" documentId="6_{4F45DE64-BE33-4F18-9BCE-C4F36FED717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E356E6B7-3246-4227-8BD7-6D96B07B54BC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Costos" sheetId="19" r:id="rId5"/>
     <sheet name="Proveedor B" sheetId="20" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -663,14 +663,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <sz val="7"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,14 +699,8 @@
         <fgColor rgb="FF1F4E79"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -786,33 +779,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -822,7 +794,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -946,12 +918,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Encabezado 1" xfId="2" builtinId="16"/>
@@ -959,7 +930,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título" xfId="3" builtinId="15"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1296,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1354,7 +1346,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="50"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1386,70 +1378,74 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="63">
-        <v>1920</v>
-      </c>
-      <c r="C6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="D6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="E6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="F6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="G6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="H6" s="64">
-        <v>1920</v>
-      </c>
-      <c r="I6" s="64">
-        <v>1920</v>
+        <v>1864</v>
+      </c>
+      <c r="C6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="D6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="E6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="F6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="G6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="H6" s="63">
+        <v>1864</v>
+      </c>
+      <c r="I6" s="63">
+        <v>1864</v>
       </c>
       <c r="J6" s="7">
         <f>SUM(B6:I6)</f>
-        <v>15360</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="63">
-        <v>750</v>
-      </c>
-      <c r="C7" s="64">
-        <v>750</v>
-      </c>
-      <c r="D7" s="64">
-        <v>750</v>
-      </c>
-      <c r="E7" s="64">
-        <v>750</v>
-      </c>
-      <c r="F7" s="64">
-        <v>750</v>
-      </c>
-      <c r="G7" s="64">
-        <v>750</v>
-      </c>
-      <c r="H7" s="64">
-        <v>750</v>
-      </c>
-      <c r="I7" s="64">
-        <v>750</v>
+      <c r="B7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="D7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="E7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="F7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="G7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="H7" s="48">
+        <v>1164</v>
+      </c>
+      <c r="I7" s="48">
+        <v>1164</v>
       </c>
       <c r="J7" s="7">
         <f>SUM(B7:I7)</f>
-        <v>6000</v>
+        <v>9312</v>
+      </c>
+      <c r="N7">
+        <f>1401/1.08</f>
+        <v>1297.2222222222222</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1517,6 +1513,13 @@
         <f>SUM(B9:I9)</f>
         <v>0</v>
       </c>
+      <c r="L9" s="63">
+        <v>1512</v>
+      </c>
+      <c r="M9">
+        <f>L9/B6</f>
+        <v>0.81115879828326176</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -1557,39 +1560,39 @@
       </c>
       <c r="B11" s="24">
         <f t="shared" ref="B11:I11" si="0">+SUM(B6:B10)</f>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="C11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="D11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="E11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="F11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="H11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="I11" s="24">
         <f t="shared" si="0"/>
-        <v>2670</v>
+        <v>3028</v>
       </c>
       <c r="J11" s="24">
         <f>+SUM(J6:J10)</f>
-        <v>21360</v>
+        <v>24224</v>
       </c>
       <c r="N11">
         <f>745*0.97</f>
@@ -1623,7 +1626,7 @@
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -1655,74 +1658,74 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="63">
-        <v>2160</v>
-      </c>
-      <c r="C15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="D15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="E15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="F15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="G15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="H15" s="64">
-        <v>2160</v>
-      </c>
-      <c r="I15" s="64">
-        <v>2160</v>
+        <v>1863</v>
+      </c>
+      <c r="C15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="D15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="E15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="F15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="G15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="H15" s="63">
+        <v>1863</v>
+      </c>
+      <c r="I15" s="63">
+        <v>1863</v>
       </c>
       <c r="J15" s="7">
         <f>SUM(B15:I15)</f>
-        <v>17280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="63">
-        <v>840</v>
-      </c>
-      <c r="C16" s="64">
-        <v>840</v>
-      </c>
-      <c r="D16" s="64">
-        <v>840</v>
-      </c>
-      <c r="E16" s="64">
-        <v>840</v>
-      </c>
-      <c r="F16" s="64">
-        <v>840</v>
-      </c>
-      <c r="G16" s="64">
-        <v>840</v>
-      </c>
-      <c r="H16" s="64">
-        <v>840</v>
-      </c>
-      <c r="I16" s="64">
-        <v>840</v>
+      <c r="B16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="C16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="D16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="E16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="F16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="G16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="H16" s="48">
+        <v>1163</v>
+      </c>
+      <c r="I16" s="48">
+        <v>1163</v>
       </c>
       <c r="J16" s="7">
         <f>SUM(B16:I16)</f>
-        <v>6720</v>
+        <v>9304</v>
       </c>
       <c r="L16">
         <f>I16*0.2</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1830,39 +1833,39 @@
       </c>
       <c r="B20" s="24">
         <f t="shared" ref="B20:J20" si="1">+SUM(B15:B19)</f>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="C20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="D20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="E20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="F20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="G20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="H20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="I20" s="24">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>3026</v>
       </c>
       <c r="J20" s="24">
         <f t="shared" si="1"/>
-        <v>24000</v>
+        <v>24208</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1892,7 +1895,7 @@
       <c r="J22" s="50"/>
       <c r="K22" s="50"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -1924,70 +1927,70 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="63">
-        <v>2029</v>
-      </c>
-      <c r="C24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="D24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="E24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="F24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="G24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="H24" s="64">
-        <v>2029</v>
-      </c>
-      <c r="I24" s="64">
-        <v>2029</v>
+        <v>1863</v>
+      </c>
+      <c r="C24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="D24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="E24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="F24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="G24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="H24" s="63">
+        <v>1863</v>
+      </c>
+      <c r="I24" s="63">
+        <v>1863</v>
       </c>
       <c r="J24" s="7">
         <f>SUM(B24:I24)</f>
-        <v>16232</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14904</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="63">
-        <v>800</v>
-      </c>
-      <c r="C25" s="64">
-        <v>800</v>
-      </c>
-      <c r="D25" s="64">
-        <v>800</v>
-      </c>
-      <c r="E25" s="64">
-        <v>800</v>
-      </c>
-      <c r="F25" s="64">
-        <v>800</v>
-      </c>
-      <c r="G25" s="64">
-        <v>800</v>
-      </c>
-      <c r="H25" s="64">
-        <v>800</v>
-      </c>
-      <c r="I25" s="64">
-        <v>800</v>
+      <c r="B25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="C25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="D25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="E25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="F25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="G25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="H25" s="48">
+        <v>1163</v>
+      </c>
+      <c r="I25" s="48">
+        <v>1163</v>
       </c>
       <c r="J25" s="7">
         <f>SUM(B25:I25)</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2095,39 +2098,39 @@
       </c>
       <c r="B29" s="24">
         <f t="shared" ref="B29:J29" si="2">+SUM(B24:B28)</f>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="C29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="D29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="E29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="F29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="G29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="H29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="I29" s="24">
         <f t="shared" si="2"/>
-        <v>2829</v>
+        <v>3026</v>
       </c>
       <c r="J29" s="24">
         <f t="shared" si="2"/>
-        <v>22632</v>
+        <v>24208</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2173,10 +2176,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="48">
-        <v>5564</v>
+        <v>19552</v>
       </c>
       <c r="C32" s="48">
-        <v>1696</v>
+        <v>14864</v>
       </c>
       <c r="D32" s="6">
         <v>0</v>
@@ -2199,10 +2202,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="48">
-        <v>1216</v>
+        <v>4467</v>
       </c>
       <c r="C33" s="48">
-        <v>1389</v>
+        <v>19</v>
       </c>
       <c r="D33" s="6">
         <v>0</v>
@@ -2225,10 +2228,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="48">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C34" s="48">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D34" s="6">
         <v>0</v>
@@ -2251,10 +2254,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="48">
-        <v>4</v>
+        <v>1380</v>
       </c>
       <c r="C35" s="48">
-        <v>0</v>
+        <v>1076</v>
       </c>
       <c r="D35" s="6">
         <v>0</v>
@@ -2277,10 +2280,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="48">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="C36" s="48">
-        <v>180</v>
+        <v>29</v>
       </c>
       <c r="D36" s="6">
         <v>0</v>
@@ -2303,10 +2306,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="48">
-        <v>158</v>
+        <v>36</v>
       </c>
       <c r="C37" s="48">
-        <v>359</v>
+        <v>58</v>
       </c>
       <c r="D37" s="6">
         <v>0</v>
@@ -2329,10 +2332,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="48">
-        <v>426</v>
+        <v>20</v>
       </c>
       <c r="C38" s="48">
-        <v>500</v>
+        <v>94</v>
       </c>
       <c r="D38" s="6">
         <v>0</v>
@@ -2355,10 +2358,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="48">
-        <v>273</v>
+        <v>46</v>
       </c>
       <c r="C39" s="48">
-        <v>375</v>
+        <v>148</v>
       </c>
       <c r="D39" s="6">
         <v>0</v>
@@ -3321,7 +3324,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>82</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>39</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>40</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>41</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
         <v>42</v>
       </c>
@@ -3391,12 +3394,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
       <c r="D102" s="11"/>
     </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="49" t="s">
         <v>84</v>
       </c>
@@ -3407,7 +3410,7 @@
       <c r="F105" s="50"/>
       <c r="G105" s="50"/>
     </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
         <v>85</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
         <v>91</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>95</v>
       </c>
@@ -3466,8 +3469,12 @@
       <c r="F108" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H108">
+        <f>B109/B107</f>
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10" t="s">
         <v>99</v>
       </c>
@@ -3487,7 +3494,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>101</v>
       </c>
@@ -3592,6 +3599,12 @@
       </c>
       <c r="B118" s="15" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E119">
+        <f>B117/B115</f>
+        <v>1.1212121212121211</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3690,7 +3703,7 @@
       </c>
       <c r="B8" s="24">
         <f>Inputs!J11</f>
-        <v>21360</v>
+        <v>24224</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -3752,7 +3765,7 @@
       </c>
       <c r="C12" s="36">
         <f>Inputs!J6</f>
-        <v>15360</v>
+        <v>14912</v>
       </c>
       <c r="D12" s="36">
         <f>Inputs!B66</f>
@@ -3772,7 +3785,7 @@
       </c>
       <c r="H12" s="36">
         <f>B12*(C12/8)</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="I12" s="36">
         <f>IF($B$6="",0,$B$5*H12*$B$6)</f>
@@ -3780,7 +3793,7 @@
       </c>
       <c r="J12" s="36">
         <f>IF(LEFT(A12,5)="Parte",H12+I12,"")</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="K12" s="1">
         <f>Inputs!$B$95</f>
@@ -3792,11 +3805,11 @@
       </c>
       <c r="M12" s="36">
         <f>IF(AND(K12&gt;0,L12&gt;0),SQRT(2*H12*K12/L12),"")</f>
-        <v>5425.8639865002142</v>
+        <v>5346.1512636038779</v>
       </c>
       <c r="N12" s="36">
         <f t="shared" ref="N12:N19" si="3">IF(M12="","",ROUNDUP(M12/D12,0))</f>
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -3809,7 +3822,7 @@
       </c>
       <c r="C13" s="36">
         <f>Inputs!J15</f>
-        <v>17280</v>
+        <v>14904</v>
       </c>
       <c r="D13" s="36">
         <f>Inputs!B67</f>
@@ -3829,7 +3842,7 @@
       </c>
       <c r="H13" s="36">
         <f>B13*(C13/8)</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="I13" s="36">
         <f t="shared" ref="I13:I19" si="4">IF($B$6="",0,$B$5*H13*$B$6)</f>
@@ -3837,7 +3850,7 @@
       </c>
       <c r="J13" s="36">
         <f>IF(LEFT(A13,5)="Parte",H13+I13,"")</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="K13" s="1">
         <f>Inputs!$B$96</f>
@@ -3849,11 +3862,11 @@
       </c>
       <c r="M13" s="36">
         <f>IF(AND(K13&gt;0,L13&gt;0),SQRT(2*H13*K13/L13),"")</f>
-        <v>1073.312629199899</v>
+        <v>996.794863550169</v>
       </c>
       <c r="N13" s="36">
         <f>IF(M13="","",ROUNDUP(M13/D13,0))</f>
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -3866,7 +3879,7 @@
       </c>
       <c r="C14" s="36">
         <f>B14*Inputs!$J$15</f>
-        <v>172.8</v>
+        <v>149.04</v>
       </c>
       <c r="D14" s="36">
         <f>Inputs!B68</f>
@@ -3882,11 +3895,11 @@
       </c>
       <c r="G14" s="36">
         <f t="shared" si="2"/>
-        <v>172.8</v>
+        <v>149.04</v>
       </c>
       <c r="H14" s="36">
-        <f t="shared" ref="H13:H19" si="5">B14*(C14/8)</f>
-        <v>0.21600000000000003</v>
+        <f t="shared" ref="H14:H19" si="5">B14*(C14/8)</f>
+        <v>0.18629999999999999</v>
       </c>
       <c r="I14" s="36">
         <f t="shared" si="4"/>
@@ -3923,7 +3936,7 @@
       </c>
       <c r="C15" s="36">
         <f>B15*Inputs!$J$15</f>
-        <v>138240</v>
+        <v>119232</v>
       </c>
       <c r="D15" s="36">
         <f>Inputs!B69</f>
@@ -3939,11 +3952,11 @@
       </c>
       <c r="G15" s="36">
         <f t="shared" si="2"/>
-        <v>138240</v>
+        <v>119232</v>
       </c>
       <c r="H15" s="36">
         <f t="shared" si="5"/>
-        <v>138240</v>
+        <v>119232</v>
       </c>
       <c r="I15" s="36">
         <f t="shared" si="4"/>
@@ -3980,7 +3993,7 @@
       </c>
       <c r="C16" s="36">
         <f>B16*Inputs!$J$24</f>
-        <v>4869.5999999999995</v>
+        <v>4471.2</v>
       </c>
       <c r="D16" s="36">
         <f>Inputs!B70</f>
@@ -3996,11 +4009,11 @@
       </c>
       <c r="G16" s="36">
         <f t="shared" si="2"/>
-        <v>4869.5999999999995</v>
+        <v>4471.2</v>
       </c>
       <c r="H16" s="36">
         <f t="shared" si="5"/>
-        <v>182.60999999999999</v>
+        <v>167.67</v>
       </c>
       <c r="I16" s="36">
         <f t="shared" si="4"/>
@@ -4037,7 +4050,7 @@
       </c>
       <c r="C17" s="36">
         <f>B17*Inputs!$J$24</f>
-        <v>9739.1999999999989</v>
+        <v>8942.4</v>
       </c>
       <c r="D17" s="36">
         <f>Inputs!B71</f>
@@ -4053,11 +4066,11 @@
       </c>
       <c r="G17" s="36">
         <f t="shared" si="2"/>
-        <v>9739.1999999999989</v>
+        <v>8942.4</v>
       </c>
       <c r="H17" s="36">
         <f t="shared" si="5"/>
-        <v>730.43999999999994</v>
+        <v>670.68</v>
       </c>
       <c r="I17" s="36">
         <f t="shared" si="4"/>
@@ -4094,7 +4107,7 @@
       </c>
       <c r="C18" s="36">
         <f>B18*Inputs!$J$24</f>
-        <v>32464</v>
+        <v>29808</v>
       </c>
       <c r="D18" s="36">
         <f>Inputs!B72</f>
@@ -4110,11 +4123,11 @@
       </c>
       <c r="G18" s="36">
         <f t="shared" si="2"/>
-        <v>32464</v>
+        <v>29808</v>
       </c>
       <c r="H18" s="36">
         <f t="shared" si="5"/>
-        <v>8116</v>
+        <v>7452</v>
       </c>
       <c r="I18" s="36">
         <f t="shared" si="4"/>
@@ -4151,7 +4164,7 @@
       </c>
       <c r="C19" s="36">
         <f>B19*Inputs!$J$24</f>
-        <v>12174</v>
+        <v>11178</v>
       </c>
       <c r="D19" s="36">
         <f>Inputs!B73</f>
@@ -4167,11 +4180,11 @@
       </c>
       <c r="G19" s="36">
         <f t="shared" si="2"/>
-        <v>12174</v>
+        <v>11178</v>
       </c>
       <c r="H19" s="36">
         <f t="shared" si="5"/>
-        <v>1141.3125</v>
+        <v>1047.9375</v>
       </c>
       <c r="I19" s="36">
         <f t="shared" si="4"/>
@@ -4257,7 +4270,7 @@
       </c>
       <c r="C23" s="36">
         <f>Inputs!J7</f>
-        <v>6000</v>
+        <v>9312</v>
       </c>
       <c r="D23" s="36">
         <f>Inputs!B66</f>
@@ -4277,7 +4290,7 @@
       </c>
       <c r="H23" s="36">
         <f>B23*(C23/8)</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="I23" s="36">
         <f>IF($B$6="",0,$B$5*H23*$B$6)</f>
@@ -4285,7 +4298,7 @@
       </c>
       <c r="J23" s="36">
         <f>IF(LEFT(A23,5)="Parte",H23+I23,"")</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="K23" s="1">
         <f>Inputs!$B$95</f>
@@ -4297,11 +4310,11 @@
       </c>
       <c r="M23" s="36">
         <f t="shared" ref="M23:M30" si="9">IF(AND(K23&gt;0,L23&gt;0),SQRT(2*H23*K23/L23),"")</f>
-        <v>3391.164991562634</v>
+        <v>4224.6893376909975</v>
       </c>
       <c r="N23" s="36">
         <f t="shared" ref="N23:N30" si="10">IF(M23="","",ROUNDUP(M23/D23,0))</f>
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -4314,7 +4327,7 @@
       </c>
       <c r="C24" s="36">
         <f>Inputs!J16</f>
-        <v>6720</v>
+        <v>9304</v>
       </c>
       <c r="D24" s="36">
         <f>Inputs!B67</f>
@@ -4334,7 +4347,7 @@
       </c>
       <c r="H24" s="36">
         <f t="shared" ref="H24:H30" si="13">B24*(C24/8)</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="I24" s="36">
         <f>IF($B$6="",0,$B$5*H24*$B$6)</f>
@@ -4342,7 +4355,7 @@
       </c>
       <c r="J24" s="36">
         <f>IF(LEFT(A24,5)="Parte",H24+I24,"")</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="K24" s="1">
         <f>Inputs!$B$96</f>
@@ -4354,11 +4367,11 @@
       </c>
       <c r="M24" s="36">
         <f t="shared" si="9"/>
-        <v>669.32802122726048</v>
+        <v>787.57010269985915</v>
       </c>
       <c r="N24" s="36">
         <f t="shared" si="10"/>
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -4371,7 +4384,7 @@
       </c>
       <c r="C25" s="36">
         <f>B25*Inputs!$J$16</f>
-        <v>67.2</v>
+        <v>93.04</v>
       </c>
       <c r="D25" s="36">
         <f>Inputs!B68</f>
@@ -4387,11 +4400,11 @@
       </c>
       <c r="G25" s="36">
         <f>IF(LEFT(A25,5)="Pieza",C25+F25,"")</f>
-        <v>67.2</v>
+        <v>93.04</v>
       </c>
       <c r="H25" s="36">
         <f t="shared" si="13"/>
-        <v>8.4000000000000005E-2</v>
+        <v>0.11630000000000001</v>
       </c>
       <c r="I25" s="36">
         <f t="shared" ref="I25:I30" si="14">IF($B$6="",0,$B$5*H25*$B$6)</f>
@@ -4427,7 +4440,7 @@
       </c>
       <c r="C26" s="36">
         <f>B26*Inputs!$J$25</f>
-        <v>51200</v>
+        <v>74432</v>
       </c>
       <c r="D26" s="36">
         <f>Inputs!B69</f>
@@ -4443,11 +4456,11 @@
       </c>
       <c r="G26" s="36">
         <f>IF(LEFT(A26,5)="Pieza",C26+F26,"")</f>
-        <v>51200</v>
+        <v>74432</v>
       </c>
       <c r="H26" s="36">
         <f t="shared" si="13"/>
-        <v>51200</v>
+        <v>74432</v>
       </c>
       <c r="I26" s="36">
         <f t="shared" si="14"/>
@@ -4484,7 +4497,7 @@
       </c>
       <c r="C27" s="36">
         <f>B27*Inputs!$J$25</f>
-        <v>1920</v>
+        <v>2791.2</v>
       </c>
       <c r="D27" s="36">
         <f>Inputs!B70</f>
@@ -4500,11 +4513,11 @@
       </c>
       <c r="G27" s="36">
         <f t="shared" si="8"/>
-        <v>1920</v>
+        <v>2791.2</v>
       </c>
       <c r="H27" s="36">
         <f t="shared" si="13"/>
-        <v>72</v>
+        <v>104.66999999999999</v>
       </c>
       <c r="I27" s="36">
         <f t="shared" si="14"/>
@@ -4541,7 +4554,7 @@
       </c>
       <c r="C28" s="36">
         <f>B28*Inputs!$J$25</f>
-        <v>3840</v>
+        <v>5582.4</v>
       </c>
       <c r="D28" s="36">
         <f>Inputs!B71</f>
@@ -4557,11 +4570,11 @@
       </c>
       <c r="G28" s="36">
         <f t="shared" si="8"/>
-        <v>3840</v>
+        <v>5582.4</v>
       </c>
       <c r="H28" s="36">
         <f t="shared" si="13"/>
-        <v>288</v>
+        <v>418.67999999999995</v>
       </c>
       <c r="I28" s="36">
         <f t="shared" si="14"/>
@@ -4598,7 +4611,7 @@
       </c>
       <c r="C29" s="36">
         <f>B29*Inputs!$J$25</f>
-        <v>12800</v>
+        <v>18608</v>
       </c>
       <c r="D29" s="36">
         <f>Inputs!B72</f>
@@ -4614,11 +4627,11 @@
       </c>
       <c r="G29" s="36">
         <f t="shared" si="8"/>
-        <v>12800</v>
+        <v>18608</v>
       </c>
       <c r="H29" s="36">
         <f t="shared" si="13"/>
-        <v>3200</v>
+        <v>4652</v>
       </c>
       <c r="I29" s="36">
         <f t="shared" si="14"/>
@@ -4655,7 +4668,7 @@
       </c>
       <c r="C30" s="36">
         <f>B30*Inputs!$J$25</f>
-        <v>4800</v>
+        <v>6978</v>
       </c>
       <c r="D30" s="36">
         <f>Inputs!B73</f>
@@ -4671,11 +4684,11 @@
       </c>
       <c r="G30" s="36">
         <f t="shared" si="8"/>
-        <v>4800</v>
+        <v>6978</v>
       </c>
       <c r="H30" s="36">
         <f t="shared" si="13"/>
-        <v>450</v>
+        <v>654.1875</v>
       </c>
       <c r="I30" s="36">
         <f t="shared" si="14"/>
@@ -6221,10 +6234,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6236,7 +6249,7 @@
     <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>123</v>
       </c>
@@ -6252,7 +6265,7 @@
       <c r="K1" s="50"/>
       <c r="L1" s="50"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
         <v>124</v>
       </c>
@@ -6268,7 +6281,7 @@
       <c r="K2" s="50"/>
       <c r="L2" s="50"/>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>125</v>
       </c>
@@ -6284,12 +6297,12 @@
       <c r="K3" s="50"/>
       <c r="L3" s="50"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>21</v>
       </c>
@@ -6339,7 +6352,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>33</v>
       </c>
@@ -6349,39 +6362,39 @@
       </c>
       <c r="C6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="D6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="E6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="F6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="G6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="H6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="I6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="J6" s="18">
         <f>Inputs!$B$15*$B$6</f>
-        <v>21.6</v>
+        <v>18.63</v>
       </c>
       <c r="K6" s="19">
         <f>Inputs!J6*B6</f>
-        <v>153.6</v>
+        <v>149.12</v>
       </c>
       <c r="L6" s="39">
         <f>Politica_Inventarios!F14</f>
@@ -6389,22 +6402,22 @@
       </c>
       <c r="M6" s="24">
         <f>Inputs!B34</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="N6" s="24">
         <f>K6+L6-M6</f>
-        <v>142.6</v>
+        <v>147.12</v>
       </c>
       <c r="O6" s="39">
         <f>IF(ROUNDUP(N6/Inputs!$B$68,0)&lt;0,0,ROUNDUP(N6/Inputs!$B$68,0))+1</f>
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="P6" s="28">
         <f>O6*Inputs!$B$85</f>
-        <v>8640</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8940</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>34</v>
       </c>
@@ -6414,39 +6427,39 @@
       </c>
       <c r="C7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="D7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="E7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="F7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="G7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="H7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="I7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="J7" s="18">
         <f>Inputs!$B$24*$B$7</f>
-        <v>16232</v>
+        <v>14904</v>
       </c>
       <c r="K7" s="19">
         <f>SUM(C7:J7)</f>
-        <v>129856</v>
+        <v>119232</v>
       </c>
       <c r="L7" s="39">
         <f>Politica_Inventarios!F15</f>
@@ -6454,22 +6467,22 @@
       </c>
       <c r="M7" s="24">
         <f>Inputs!B35</f>
-        <v>4</v>
+        <v>1380</v>
       </c>
       <c r="N7" s="24">
         <f>K7+L7-M7</f>
-        <v>129852</v>
+        <v>117852</v>
       </c>
       <c r="O7" s="39">
         <f>IF(ROUNDUP(N7/Inputs!$B$69,0)&lt;0,0,ROUNDUP(N7/Inputs!$B$69,0))</f>
-        <v>1299</v>
+        <v>1179</v>
       </c>
       <c r="P7" s="28">
         <f>O7*Inputs!$B$86</f>
-        <v>9093</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
@@ -6479,39 +6492,39 @@
       </c>
       <c r="C8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="D8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="E8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="F8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="G8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="H8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="I8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="J8" s="18">
         <f>Inputs!$B$24*$B$8</f>
-        <v>608.69999999999993</v>
+        <v>558.9</v>
       </c>
       <c r="K8" s="19">
         <f>Inputs!$J$24*B8</f>
-        <v>4869.5999999999995</v>
+        <v>4471.2</v>
       </c>
       <c r="L8" s="39">
         <f>Politica_Inventarios!F16</f>
@@ -6519,22 +6532,22 @@
       </c>
       <c r="M8" s="24">
         <f>Inputs!B36</f>
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="N8" s="24">
         <f t="shared" ref="N8:N11" si="0">K8+L8-M8</f>
-        <v>4730.5999999999995</v>
+        <v>4453.2</v>
       </c>
       <c r="O8" s="39">
         <f>IF(ROUNDUP(N8/Inputs!$B$70,0)&lt;0,0,ROUNDUP(N8/Inputs!$B$70,0))</f>
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="P8" s="28">
         <f>O8*Inputs!$B$87</f>
-        <v>5688</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -6544,39 +6557,39 @@
       </c>
       <c r="C9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="D9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="E9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="F9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="G9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="H9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="I9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="J9" s="18">
         <f>Inputs!$B$24*$B$9</f>
-        <v>1217.3999999999999</v>
+        <v>1117.8</v>
       </c>
       <c r="K9" s="19">
         <f>Inputs!$J$24*B9</f>
-        <v>9739.1999999999989</v>
+        <v>8942.4</v>
       </c>
       <c r="L9" s="39">
         <f>Politica_Inventarios!F17</f>
@@ -6584,22 +6597,26 @@
       </c>
       <c r="M9" s="24">
         <f>Inputs!B37</f>
-        <v>158</v>
+        <v>36</v>
       </c>
       <c r="N9" s="24">
         <f t="shared" si="0"/>
-        <v>9581.1999999999989</v>
+        <v>8906.4</v>
       </c>
       <c r="O9" s="39">
         <f>IF(ROUNDUP(N9/Inputs!$B$71,0)&lt;0,0,ROUNDUP(N9/Inputs!$B$71,0))</f>
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="P9" s="28">
         <f>O9*Inputs!$B$88</f>
-        <v>3840</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3576</v>
+      </c>
+      <c r="S9" s="24">
+        <f>R11-R12</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
@@ -6609,39 +6626,39 @@
       </c>
       <c r="C10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="D10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="E10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="F10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="G10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="H10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="I10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="J10" s="18">
         <f>Inputs!$B$24*$B$10</f>
-        <v>4058</v>
+        <v>3726</v>
       </c>
       <c r="K10" s="19">
         <f>Inputs!$J$24*B10</f>
-        <v>32464</v>
+        <v>29808</v>
       </c>
       <c r="L10" s="39">
         <f>Politica_Inventarios!F18</f>
@@ -6649,22 +6666,22 @@
       </c>
       <c r="M10" s="24">
         <f>Inputs!B38</f>
-        <v>426</v>
+        <v>20</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="0"/>
-        <v>32038</v>
+        <v>29788</v>
       </c>
       <c r="O10" s="39">
         <f>IF(ROUNDUP(N10/Inputs!$B$72,0)&lt;0,0,ROUNDUP(N10/Inputs!$B$72,0))</f>
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="P10" s="28">
         <f>O10*Inputs!$B$89</f>
-        <v>9630</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8940</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
@@ -6674,39 +6691,39 @@
       </c>
       <c r="C11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="D11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="E11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="F11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="G11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="H11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="I11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="J11" s="18">
         <f>Inputs!$B$24*$B$11</f>
-        <v>1521.75</v>
+        <v>1397.25</v>
       </c>
       <c r="K11" s="19">
         <f>Inputs!$J$24*B11</f>
-        <v>12174</v>
+        <v>11178</v>
       </c>
       <c r="L11" s="39">
         <f>Politica_Inventarios!F19</f>
@@ -6714,75 +6731,94 @@
       </c>
       <c r="M11" s="24">
         <f>Inputs!B39</f>
-        <v>273</v>
+        <v>46</v>
       </c>
       <c r="N11" s="24">
         <f t="shared" si="0"/>
-        <v>11901</v>
+        <v>11132</v>
       </c>
       <c r="O11" s="39">
         <f>IF(ROUNDUP(N11/Inputs!$B$73,0)&lt;0,0,ROUNDUP(N11/Inputs!$B$73,0))</f>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="P11" s="28">
         <f>O11*Inputs!$B$90</f>
-        <v>2240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2100</v>
+      </c>
+      <c r="R11" s="65">
+        <v>3732</v>
+      </c>
+      <c r="W11" s="65">
+        <v>14928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="20">
         <f>Inputs!B6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="D12" s="20">
         <f>Inputs!C6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="E12" s="20">
         <f>Inputs!D6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="F12" s="20">
         <f>Inputs!E6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="G12" s="20">
         <f>Inputs!F6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="H12" s="20">
         <f>Inputs!G6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="I12" s="20">
         <f>Inputs!H6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="J12" s="20">
         <f>Inputs!I6</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="K12" s="20">
         <f>Inputs!J6</f>
-        <v>15360</v>
+        <v>14912</v>
       </c>
       <c r="N12" s="24"/>
       <c r="P12" s="28">
         <f>SUM(P6:P11)</f>
-        <v>39131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>37173</v>
+      </c>
+      <c r="R12" s="48">
+        <v>3696</v>
+      </c>
+      <c r="V12" s="65">
+        <v>117900</v>
+      </c>
+      <c r="W12" s="48">
+        <v>14784</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="V14" s="24">
+        <f>W11-W12</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
@@ -6832,7 +6868,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
@@ -6841,39 +6877,39 @@
       </c>
       <c r="C16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="D16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="E16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="F16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="G16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="H16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="I16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="J16" s="18">
         <f>Inputs!$B$16*$B$16</f>
-        <v>8.4</v>
+        <v>11.63</v>
       </c>
       <c r="K16" s="19">
         <f t="shared" ref="K16:K21" si="1">SUM(C16:J16)</f>
-        <v>67.2</v>
+        <v>93.039999999999992</v>
       </c>
       <c r="L16" s="39">
         <f>Politica_Inventarios!F25</f>
@@ -6881,22 +6917,26 @@
       </c>
       <c r="M16" s="24">
         <f>Inputs!C34</f>
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="N16" s="46">
         <f>K16+L16-M16</f>
-        <v>46.2</v>
+        <v>92.039999999999992</v>
       </c>
       <c r="O16" s="39">
         <f>IF(ROUNDUP(N16/Inputs!$B$68,0)&lt;0,0,ROUNDUP(N16/Inputs!$B$68,0))+1</f>
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="P16" s="28">
         <f>O16*Inputs!$B$85</f>
-        <v>2880</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+        <v>5640</v>
+      </c>
+      <c r="T16" s="24">
+        <f>298+S9</f>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>34</v>
       </c>
@@ -6905,39 +6945,39 @@
       </c>
       <c r="C17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="D17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="E17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="F17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="G17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="H17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="I17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="J17" s="18">
         <f>Inputs!$B$25*$B$17</f>
-        <v>6400</v>
+        <v>9304</v>
       </c>
       <c r="K17" s="19">
         <f t="shared" si="1"/>
-        <v>51200</v>
+        <v>74432</v>
       </c>
       <c r="L17" s="39">
         <f>Politica_Inventarios!F26</f>
@@ -6945,22 +6985,22 @@
       </c>
       <c r="M17" s="24">
         <f>Inputs!C35</f>
-        <v>0</v>
+        <v>1076</v>
       </c>
       <c r="N17" s="24">
         <f>K17+L17-M17</f>
-        <v>51200</v>
+        <v>73356</v>
       </c>
       <c r="O17" s="39">
         <f>IF(ROUNDUP(N17/Inputs!$B$69,0)&lt;0,0,ROUNDUP(N17/Inputs!$B$69,0))</f>
-        <v>512</v>
+        <v>734</v>
       </c>
       <c r="P17" s="28">
         <f>O17*Inputs!$B$86</f>
-        <v>3584</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+        <v>5138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
@@ -6969,39 +7009,39 @@
       </c>
       <c r="C18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="D18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="E18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="F18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="G18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="H18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="I18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="J18" s="18">
         <f>Inputs!$B$25*$B$18</f>
-        <v>240</v>
+        <v>348.9</v>
       </c>
       <c r="K18" s="19">
         <f t="shared" si="1"/>
-        <v>1920</v>
+        <v>2791.2000000000003</v>
       </c>
       <c r="L18" s="39">
         <f>Politica_Inventarios!F27</f>
@@ -7009,22 +7049,26 @@
       </c>
       <c r="M18" s="24">
         <f>Inputs!C36</f>
-        <v>180</v>
+        <v>29</v>
       </c>
       <c r="N18" s="24">
         <f t="shared" ref="N18:N21" si="2">K18+L18-M18</f>
-        <v>1740</v>
+        <v>2762.2000000000003</v>
       </c>
       <c r="O18" s="39">
         <f>IF(ROUNDUP(N18/Inputs!$B$70,0)&lt;0,0,ROUNDUP(N18/Inputs!$B$70,0))</f>
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="P18" s="28">
         <f>O18*Inputs!$B$87</f>
-        <v>2088</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+        <v>3348</v>
+      </c>
+      <c r="V18" s="24">
+        <f>V12+V14</f>
+        <v>118044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>36</v>
       </c>
@@ -7033,39 +7077,39 @@
       </c>
       <c r="C19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="D19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="E19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="F19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="G19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="H19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="I19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="J19" s="18">
         <f>Inputs!$B$25*$B$19</f>
-        <v>480</v>
+        <v>697.8</v>
       </c>
       <c r="K19" s="19">
         <f t="shared" si="1"/>
-        <v>3840</v>
+        <v>5582.4000000000005</v>
       </c>
       <c r="L19" s="39">
         <f>Politica_Inventarios!F28</f>
@@ -7073,22 +7117,26 @@
       </c>
       <c r="M19" s="24">
         <f>Inputs!C37</f>
-        <v>359</v>
+        <v>58</v>
       </c>
       <c r="N19" s="24">
         <f t="shared" si="2"/>
-        <v>3481</v>
+        <v>5524.4000000000005</v>
       </c>
       <c r="O19" s="39">
         <f>IF(ROUNDUP(N19/Inputs!$B$71,0)&lt;0,0,ROUNDUP(N19/Inputs!$B$71,0))</f>
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="P19" s="28">
         <f>O19*Inputs!$B$88</f>
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+        <v>2232</v>
+      </c>
+      <c r="R19">
+        <f>117900/8</f>
+        <v>14737.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>37</v>
       </c>
@@ -7097,39 +7145,39 @@
       </c>
       <c r="C20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="D20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="E20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="F20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="G20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="H20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="I20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="J20" s="18">
         <f>Inputs!$B$25*$B$20</f>
-        <v>1600</v>
+        <v>2326</v>
       </c>
       <c r="K20" s="19">
         <f t="shared" si="1"/>
-        <v>12800</v>
+        <v>18608</v>
       </c>
       <c r="L20" s="39">
         <f>Politica_Inventarios!F29</f>
@@ -7137,22 +7185,26 @@
       </c>
       <c r="M20" s="24">
         <f>Inputs!C38</f>
-        <v>500</v>
+        <v>94</v>
       </c>
       <c r="N20" s="24">
         <f t="shared" si="2"/>
-        <v>12300</v>
+        <v>18514</v>
       </c>
       <c r="O20" s="39">
         <f>IF(ROUNDUP(N20/Inputs!$B$72,0)&lt;0,0,ROUNDUP(N20/Inputs!$B$72,0))</f>
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="P20" s="28">
         <f>O20*Inputs!$B$89</f>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+        <v>5580</v>
+      </c>
+      <c r="V20">
+        <f>+V18/8</f>
+        <v>14755.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
@@ -7161,39 +7213,39 @@
       </c>
       <c r="C21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="D21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="E21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="F21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="G21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="H21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="I21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="J21" s="18">
         <f>Inputs!$B$25*$B$21</f>
-        <v>600</v>
+        <v>872.25</v>
       </c>
       <c r="K21" s="19">
         <f t="shared" si="1"/>
-        <v>4800</v>
+        <v>6978</v>
       </c>
       <c r="L21" s="39">
         <f>Politica_Inventarios!F30</f>
@@ -7201,74 +7253,74 @@
       </c>
       <c r="M21" s="24">
         <f>Inputs!C39</f>
-        <v>375</v>
+        <v>148</v>
       </c>
       <c r="N21" s="24">
         <f t="shared" si="2"/>
-        <v>4425</v>
+        <v>6830</v>
       </c>
       <c r="O21" s="39">
         <f>IF(ROUNDUP(N21/Inputs!$B$73,0)&lt;0,0,ROUNDUP(N21/Inputs!$B$73,0))</f>
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="P21" s="28">
         <f>O21*Inputs!$B$90</f>
-        <v>840</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="20">
         <f>Inputs!B7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="D22" s="20">
         <f>Inputs!C7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="E22" s="20">
         <f>Inputs!D7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="F22" s="20">
         <f>Inputs!E7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="G22" s="20">
         <f>Inputs!F7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="H22" s="20">
         <f>Inputs!G7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="I22" s="20">
         <f>Inputs!H7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="J22" s="20">
         <f>Inputs!I7</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="K22" s="20">
         <f>Inputs!J7</f>
-        <v>6000</v>
+        <v>9312</v>
       </c>
       <c r="P22" s="28">
         <f>SUM(P16:P21)</f>
-        <v>14498</v>
+        <v>23226</v>
       </c>
       <c r="R22" s="28"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>21</v>
       </c>
@@ -7318,7 +7370,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
@@ -7382,7 +7434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
@@ -7446,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
@@ -7510,7 +7562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>36</v>
       </c>
@@ -7574,7 +7626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
@@ -7638,7 +7690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>38</v>
       </c>
@@ -7702,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>127</v>
       </c>
@@ -8721,7 +8773,7 @@
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P54" s="28">
         <f>SUM(P12,P22,P32,P42)</f>
-        <v>53629</v>
+        <v>60399</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
@@ -8742,8 +8794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="J3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8943,43 +8995,43 @@
       </c>
       <c r="B7" s="21">
         <f>Inputs!B32</f>
-        <v>5564</v>
+        <v>19552</v>
       </c>
       <c r="C7" s="16">
         <f t="shared" ref="C7:I7" si="0">B10</f>
-        <v>3644</v>
+        <v>17688</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
-        <v>1724</v>
+        <v>15824</v>
       </c>
       <c r="E7" s="16">
         <f t="shared" si="0"/>
-        <v>5234</v>
+        <v>13960</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" si="0"/>
-        <v>3314</v>
+        <v>12096</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>1394</v>
+        <v>10232</v>
       </c>
       <c r="H7" s="16">
         <f t="shared" si="0"/>
-        <v>4904</v>
+        <v>8368</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="0"/>
-        <v>2984</v>
+        <v>6504</v>
       </c>
       <c r="J7" s="39">
         <f>Politica_Inventarios!N12</f>
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K7" s="39">
         <f>Politica_Inventarios!J12</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="L7" s="39">
         <f>Inputs!B66</f>
@@ -8990,43 +9042,43 @@
       </c>
       <c r="P7" s="21">
         <f>Inputs!B33</f>
-        <v>1216</v>
+        <v>4467</v>
       </c>
       <c r="Q7" s="16">
         <f t="shared" ref="Q7:W7" si="1">P10</f>
-        <v>784</v>
+        <v>4094.4</v>
       </c>
       <c r="R7" s="16">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>3721.8</v>
       </c>
       <c r="S7" s="16">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>3349.2000000000003</v>
       </c>
       <c r="T7" s="16">
         <f t="shared" si="1"/>
-        <v>568</v>
+        <v>2976.6000000000004</v>
       </c>
       <c r="U7" s="16">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>2604.0000000000005</v>
       </c>
       <c r="V7" s="16">
         <f t="shared" si="1"/>
-        <v>784</v>
+        <v>2231.4000000000005</v>
       </c>
       <c r="W7" s="16">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>1858.8000000000006</v>
       </c>
       <c r="X7" s="39">
         <f>Politica_Inventarios!N13</f>
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Y7" s="39">
         <f>Politica_Inventarios!J13</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="Z7" s="24">
         <f>Inputs!B67</f>
@@ -9044,7 +9096,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="6">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -9053,7 +9105,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -9063,7 +9115,7 @@
       </c>
       <c r="M8" s="28">
         <f>SUM(B8:I8)*VLOOKUP(Inputs!B110,Inputs!A107:B109,2,FALSE)</f>
-        <v>45250</v>
+        <v>0</v>
       </c>
       <c r="O8" s="9" t="s">
         <v>136</v>
@@ -9075,7 +9127,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="S8" s="6">
         <v>0</v>
@@ -9084,17 +9136,17 @@
         <v>0</v>
       </c>
       <c r="U8" s="6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="V8" s="6">
         <v>0</v>
       </c>
       <c r="W8" s="6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="1">
         <f>SUM(P8:W8)*VLOOKUP(Inputs!B118,Inputs!A114:B117,2,FALSE)</f>
-        <v>89100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9103,78 +9155,83 @@
       </c>
       <c r="B9" s="21">
         <f>Inputs!B6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="C9" s="21">
         <f>Inputs!C6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="D9" s="21">
         <f>Inputs!D6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="E9" s="21">
         <f>Inputs!E6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="F9" s="21">
         <f>Inputs!F6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="G9" s="21">
         <f>Inputs!G6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="H9" s="21">
         <f>Inputs!H6*Inputs!$B$48</f>
-        <v>1920</v>
+        <v>1864</v>
       </c>
       <c r="I9" s="21">
         <f>Inputs!I6*Inputs!$B$48</f>
-        <v>1920</v>
-      </c>
-      <c r="K9">
-        <f>J7/2</f>
-        <v>90.5</v>
-      </c>
+        <v>1864</v>
+      </c>
+      <c r="J9" s="24">
+        <f>SUM(B9:I9)-I10</f>
+        <v>10272</v>
+      </c>
+      <c r="K9" s="24"/>
       <c r="O9" s="9" t="s">
         <v>137</v>
       </c>
       <c r="P9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="Q9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="R9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="S9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="T9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="U9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="V9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
       </c>
       <c r="W9" s="21">
         <f>Inputs!$B$15*Inputs!$B$49</f>
-        <v>432</v>
+        <v>372.6</v>
+      </c>
+      <c r="X9" s="24">
+        <f>SUM(P9:W9)-W10</f>
+        <v>1494.599999999999</v>
       </c>
       <c r="Y9">
         <f>X7/2</f>
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9183,70 +9240,84 @@
       </c>
       <c r="B10" s="19">
         <f>B7+(B8*$L$7)-B9</f>
-        <v>3644</v>
+        <v>17688</v>
       </c>
       <c r="C10" s="19">
         <f t="shared" ref="C10:I10" si="2">C7+(C8*$L$7)-C9</f>
-        <v>1724</v>
+        <v>15824</v>
       </c>
       <c r="D10" s="19">
         <f t="shared" si="2"/>
-        <v>5234</v>
+        <v>13960</v>
       </c>
       <c r="E10" s="19">
         <f t="shared" si="2"/>
-        <v>3314</v>
+        <v>12096</v>
       </c>
       <c r="F10" s="19">
         <f t="shared" si="2"/>
-        <v>1394</v>
+        <v>10232</v>
       </c>
       <c r="G10" s="19">
         <f t="shared" si="2"/>
-        <v>4904</v>
+        <v>8368</v>
       </c>
       <c r="H10" s="19">
         <f t="shared" si="2"/>
-        <v>2984</v>
+        <v>6504</v>
       </c>
       <c r="I10" s="19">
         <f t="shared" si="2"/>
-        <v>1064</v>
+        <v>4640</v>
+      </c>
+      <c r="J10">
+        <v>380.8</v>
+      </c>
+      <c r="K10" s="64">
+        <f>J9/L7</f>
+        <v>342.4</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>138</v>
       </c>
       <c r="P10" s="19">
         <f>P7+(P8*$Z$7)-P9</f>
-        <v>784</v>
+        <v>4094.4</v>
       </c>
       <c r="Q10" s="19">
         <f t="shared" ref="Q10:W10" si="3">Q7+(Q8*$Z$7)-Q9</f>
-        <v>352</v>
+        <v>3721.8</v>
       </c>
       <c r="R10" s="19">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>3349.2000000000003</v>
       </c>
       <c r="S10" s="19">
         <f>S7+(S8*$Z$7)-S9</f>
-        <v>568</v>
+        <v>2976.6000000000004</v>
       </c>
       <c r="T10" s="19">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>2604.0000000000005</v>
       </c>
       <c r="U10" s="19">
         <f t="shared" si="3"/>
-        <v>784</v>
+        <v>2231.4000000000005</v>
       </c>
       <c r="V10" s="19">
         <f t="shared" si="3"/>
-        <v>352</v>
+        <v>1858.8000000000006</v>
       </c>
       <c r="W10" s="19">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1486.2000000000007</v>
+      </c>
+      <c r="X10">
+        <v>144</v>
+      </c>
+      <c r="Y10" s="64">
+        <f>X9/Z7</f>
+        <v>124.54999999999991</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9335,43 +9406,43 @@
       </c>
       <c r="B13" s="21">
         <f>Inputs!C32</f>
-        <v>1696</v>
+        <v>14864</v>
       </c>
       <c r="C13" s="16">
         <f t="shared" ref="C13:I13" si="4">B16</f>
-        <v>4246</v>
+        <v>13700</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="4"/>
-        <v>3496</v>
+        <v>12536</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="4"/>
-        <v>6046</v>
+        <v>11372</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="4"/>
-        <v>5296</v>
+        <v>10208</v>
       </c>
       <c r="G13" s="16">
         <f t="shared" si="4"/>
-        <v>7846</v>
+        <v>9044</v>
       </c>
       <c r="H13" s="16">
         <f t="shared" si="4"/>
-        <v>7096</v>
+        <v>7880</v>
       </c>
       <c r="I13" s="16">
         <f t="shared" si="4"/>
-        <v>6346</v>
+        <v>6716</v>
       </c>
       <c r="J13" s="39">
         <f>Politica_Inventarios!N23</f>
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="K13" s="39">
         <f>Politica_Inventarios!J23</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="L13">
         <v>30</v>
@@ -9380,44 +9451,44 @@
         <v>135</v>
       </c>
       <c r="P13" s="21">
-        <f>Inputs!C33</f>
-        <v>1389</v>
+        <f>Inputs!C32</f>
+        <v>14864</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" ref="Q13:W13" si="5">P16</f>
-        <v>1221</v>
+        <v>15435.4</v>
       </c>
       <c r="R13" s="16">
         <f t="shared" si="5"/>
-        <v>1053</v>
+        <v>15202.8</v>
       </c>
       <c r="S13" s="16">
         <f t="shared" si="5"/>
-        <v>885</v>
+        <v>14970.199999999999</v>
       </c>
       <c r="T13" s="16">
         <f t="shared" si="5"/>
-        <v>717</v>
+        <v>15541.599999999999</v>
       </c>
       <c r="U13" s="16">
         <f t="shared" si="5"/>
-        <v>549</v>
+        <v>15308.999999999998</v>
       </c>
       <c r="V13" s="16">
         <f t="shared" si="5"/>
-        <v>381</v>
+        <v>15076.399999999998</v>
       </c>
       <c r="W13" s="16">
         <f t="shared" si="5"/>
-        <v>213</v>
+        <v>15647.799999999997</v>
       </c>
       <c r="X13" s="39">
         <f>Politica_Inventarios!N24</f>
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="Y13" s="39">
         <f>Politica_Inventarios!J24</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="Z13">
         <v>12</v>
@@ -9428,19 +9499,19 @@
         <v>136</v>
       </c>
       <c r="B14" s="6">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
       </c>
       <c r="D14" s="6">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
         <v>0</v>
       </c>
       <c r="F14" s="6">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -9453,13 +9524,13 @@
       </c>
       <c r="M14" s="28">
         <f>SUM(B14:I14)*VLOOKUP(Inputs!B110,Inputs!A107:B109,2,FALSE)</f>
-        <v>41250</v>
+        <v>0</v>
       </c>
       <c r="O14" s="9" t="s">
         <v>136</v>
       </c>
       <c r="P14" s="6">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Q14" s="6">
         <v>0</v>
@@ -9468,7 +9539,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="6">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="T14" s="6">
         <v>0</v>
@@ -9477,14 +9548,14 @@
         <v>0</v>
       </c>
       <c r="V14" s="6">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="W14" s="6">
         <v>0</v>
       </c>
       <c r="AA14" s="1">
         <f>SUM(P14:W14)*VLOOKUP(Inputs!B118,Inputs!A114:B117,2,FALSE)</f>
-        <v>0</v>
+        <v>66330</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9493,78 +9564,86 @@
       </c>
       <c r="B15" s="21">
         <f>Inputs!B7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="C15" s="21">
         <f>Inputs!C7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="D15" s="21">
         <f>Inputs!D7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="E15" s="21">
         <f>Inputs!E7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="F15" s="21">
         <f>Inputs!F7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="G15" s="21">
         <f>Inputs!G7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="H15" s="21">
         <f>Inputs!H7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
       </c>
       <c r="I15" s="21">
         <f>Inputs!I7*Inputs!$B$48</f>
-        <v>750</v>
+        <v>1164</v>
+      </c>
+      <c r="J15" s="24">
+        <f>SUM(B15:I15)-I16</f>
+        <v>3760</v>
       </c>
       <c r="K15">
         <f>J13/2</f>
-        <v>57</v>
+        <v>70.5</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>137</v>
       </c>
       <c r="P15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="Q15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="R15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="S15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="T15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="U15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="V15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
       </c>
       <c r="W15" s="21">
         <f>Inputs!$B$16*Inputs!$B$49</f>
-        <v>168</v>
+        <v>232.60000000000002</v>
+      </c>
+      <c r="X15" s="24">
+        <f>SUM(P15:W15)-W16</f>
+        <v>-13554.399999999998</v>
       </c>
       <c r="Y15">
         <f>X13/2</f>
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9573,70 +9652,84 @@
       </c>
       <c r="B16" s="19">
         <f>B13+(B14*$L$13)-B15</f>
-        <v>4246</v>
+        <v>13700</v>
       </c>
       <c r="C16" s="19">
         <f t="shared" ref="C16:I16" si="6">C13+(C14*$L$7)-C15</f>
-        <v>3496</v>
+        <v>12536</v>
       </c>
       <c r="D16" s="19">
         <f t="shared" si="6"/>
-        <v>6046</v>
+        <v>11372</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="6"/>
-        <v>5296</v>
+        <v>10208</v>
       </c>
       <c r="F16" s="19">
         <f t="shared" si="6"/>
-        <v>7846</v>
+        <v>9044</v>
       </c>
       <c r="G16" s="19">
         <f t="shared" si="6"/>
-        <v>7096</v>
+        <v>7880</v>
       </c>
       <c r="H16" s="19">
         <f t="shared" si="6"/>
-        <v>6346</v>
+        <v>6716</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="6"/>
-        <v>5596</v>
+        <v>5552</v>
+      </c>
+      <c r="J16">
+        <v>149.33333333333334</v>
+      </c>
+      <c r="K16" s="64">
+        <f>J15/L13</f>
+        <v>125.33333333333333</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>138</v>
       </c>
       <c r="P16" s="19">
         <f>P13+(P14*$Z$7)-P15</f>
-        <v>1221</v>
+        <v>15435.4</v>
       </c>
       <c r="Q16" s="19">
         <f t="shared" ref="Q16:W16" si="7">Q13+(Q14*$Z$7)-Q15</f>
-        <v>1053</v>
+        <v>15202.8</v>
       </c>
       <c r="R16" s="19">
         <f t="shared" si="7"/>
-        <v>885</v>
+        <v>14970.199999999999</v>
       </c>
       <c r="S16" s="19">
         <f t="shared" si="7"/>
-        <v>717</v>
+        <v>15541.599999999999</v>
       </c>
       <c r="T16" s="19">
         <f t="shared" si="7"/>
-        <v>549</v>
+        <v>15308.999999999998</v>
       </c>
       <c r="U16" s="19">
         <f t="shared" si="7"/>
-        <v>381</v>
+        <v>15076.399999999998</v>
       </c>
       <c r="V16" s="19">
         <f t="shared" si="7"/>
-        <v>213</v>
+        <v>15647.799999999997</v>
       </c>
       <c r="W16" s="19">
         <f t="shared" si="7"/>
-        <v>45</v>
+        <v>15415.199999999997</v>
+      </c>
+      <c r="X16">
+        <v>120</v>
+      </c>
+      <c r="Y16" s="64">
+        <f>X15/Z13</f>
+        <v>-1129.5333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10723,7 +10816,7 @@
       </c>
       <c r="M35" s="28">
         <f>SUM(M14,M8)</f>
-        <v>86500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.3">
@@ -10740,74 +10833,74 @@
       </c>
       <c r="B37" s="28">
         <f>SUM(B10+B16+B22+B28+B34)*Inputs!$C$95</f>
-        <v>2367</v>
+        <v>9416.4</v>
       </c>
       <c r="C37" s="28">
         <f>SUM(C10+C16+C22+C28+C34)*Inputs!$C$95</f>
-        <v>1566</v>
+        <v>8508</v>
       </c>
       <c r="D37" s="28">
         <f>SUM(D10+D16+D22+D28+D34)*Inputs!$C$95</f>
-        <v>3384</v>
+        <v>7599.5999999999995</v>
       </c>
       <c r="E37" s="28">
         <f>SUM(E10+E16+E22+E28+E34)*Inputs!$C$95</f>
-        <v>2583</v>
+        <v>6691.2</v>
       </c>
       <c r="F37" s="28">
         <f>SUM(F10+F16+F22+F28+F34)*Inputs!$C$95</f>
-        <v>2772</v>
+        <v>5782.8</v>
       </c>
       <c r="G37" s="28">
         <f>SUM(G10+G16+G22+G28+G34)*Inputs!$C$95</f>
-        <v>3600</v>
+        <v>4874.3999999999996</v>
       </c>
       <c r="H37" s="28">
         <f>SUM(H10+H16+H22+H28+H34)*Inputs!$C$95</f>
-        <v>2799</v>
+        <v>3966</v>
       </c>
       <c r="I37" s="28">
         <f>SUM(I10+I16+I22+I28+I34)*Inputs!$C$95</f>
-        <v>1998</v>
+        <v>3057.6</v>
       </c>
       <c r="J37" s="28">
         <f>SUM(B37:I37)</f>
-        <v>21069</v>
+        <v>49896</v>
       </c>
       <c r="O37" t="s">
         <v>149</v>
       </c>
       <c r="P37" s="28">
         <f>SUM(P10+P16+P22+P28+P34)*Inputs!$C$95</f>
-        <v>601.5</v>
+        <v>5858.94</v>
       </c>
       <c r="Q37" s="28">
         <f>SUM(Q10+Q16+Q22+Q28+Q34)*Inputs!$C$95</f>
-        <v>421.5</v>
+        <v>5677.3799999999992</v>
       </c>
       <c r="R37" s="28">
         <f>SUM(R10+R16+R22+R28+R34)*Inputs!$C$95</f>
-        <v>565.5</v>
+        <v>5495.8199999999988</v>
       </c>
       <c r="S37" s="28">
         <f>SUM(S10+S16+S22+S28+S34)*Inputs!$C$95</f>
-        <v>385.5</v>
+        <v>5555.4599999999991</v>
       </c>
       <c r="T37" s="28">
         <f>SUM(T10+T16+T22+T28+T34)*Inputs!$C$95</f>
-        <v>205.5</v>
+        <v>5373.9</v>
       </c>
       <c r="U37" s="28">
         <f>SUM(U10+U16+U22+U28+U34)*Inputs!$C$95</f>
-        <v>349.5</v>
+        <v>5192.3399999999992</v>
       </c>
       <c r="V37" s="28">
         <f>SUM(V10+V16+V22+V28+V34)*Inputs!$C$95</f>
-        <v>169.5</v>
+        <v>5251.98</v>
       </c>
       <c r="W37" s="28">
         <f>SUM(W10+W16+W22+W28+W34)*Inputs!$C$95</f>
-        <v>313.5</v>
+        <v>5070.4199999999992</v>
       </c>
       <c r="X37" s="28"/>
       <c r="Z37" s="28"/>
@@ -10818,7 +10911,7 @@
       </c>
       <c r="B38" s="28">
         <f>B39*Inputs!$B$95</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="C38" s="28">
         <f>C39*Inputs!$B$95</f>
@@ -10826,7 +10919,7 @@
       </c>
       <c r="D38" s="28">
         <f>D39*Inputs!$B$95</f>
-        <v>4600</v>
+        <v>0</v>
       </c>
       <c r="E38" s="28">
         <f>E39*Inputs!$B$95</f>
@@ -10834,11 +10927,11 @@
       </c>
       <c r="F38" s="28">
         <f>F39*Inputs!$B$95</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="G38" s="28">
         <f>G39*Inputs!$B$95</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H38" s="28">
         <f>H39*Inputs!$B$95</f>
@@ -10850,14 +10943,14 @@
       </c>
       <c r="J38" s="28">
         <f>SUM(B38:I38)</f>
-        <v>11500</v>
+        <v>0</v>
       </c>
       <c r="O38" t="s">
         <v>150</v>
       </c>
       <c r="P38" s="28">
         <f>P39*Inputs!$B$96</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="Q38" s="28">
         <f>Q39*Inputs!$B$96</f>
@@ -10865,11 +10958,11 @@
       </c>
       <c r="R38" s="28">
         <f>R39*Inputs!$B$96</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="S38" s="28">
         <f>S39*Inputs!$B$96</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="T38" s="28">
         <f>T39*Inputs!$B$96</f>
@@ -10877,15 +10970,15 @@
       </c>
       <c r="U38" s="28">
         <f>U39*Inputs!$B$96</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="V38" s="28">
         <f>V39*Inputs!$B$96</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="W38" s="28">
         <f>W39*Inputs!$B$96</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="X38" s="28"/>
       <c r="Z38" s="28"/>
@@ -10896,7 +10989,7 @@
       </c>
       <c r="B39">
         <f>+COUNTIF(B42:B46,"&gt;0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <f t="shared" ref="C39:I39" si="20">+COUNTIF(C42:C46,"&gt;0")</f>
@@ -10904,7 +10997,7 @@
       </c>
       <c r="D39">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <f t="shared" si="20"/>
@@ -10912,11 +11005,11 @@
       </c>
       <c r="F39">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <f t="shared" si="20"/>
@@ -10931,7 +11024,7 @@
       </c>
       <c r="P39">
         <f>+COUNTIF(P42:P46,"&gt;0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q39">
         <f t="shared" ref="Q39:W39" si="21">+COUNTIF(Q42:Q46,"&gt;0")</f>
@@ -10939,11 +11032,11 @@
       </c>
       <c r="R39">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S39">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T39">
         <f t="shared" si="21"/>
@@ -10951,21 +11044,21 @@
       </c>
       <c r="U39">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V39">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W39">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="J40" s="28">
         <f>+SUM(J37:J38)</f>
-        <v>32569</v>
+        <v>49896</v>
       </c>
       <c r="X40" s="28"/>
     </row>
@@ -10988,7 +11081,7 @@
       </c>
       <c r="D42" s="24">
         <f t="shared" si="22"/>
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="E42" s="24">
         <f t="shared" si="22"/>
@@ -11000,7 +11093,7 @@
       </c>
       <c r="G42" s="24">
         <f t="shared" si="22"/>
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="H42" s="24">
         <f t="shared" si="22"/>
@@ -11020,7 +11113,7 @@
       </c>
       <c r="R42" s="24">
         <f t="shared" si="23"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="S42" s="24">
         <f t="shared" si="23"/>
@@ -11032,7 +11125,7 @@
       </c>
       <c r="U42" s="24">
         <f t="shared" si="23"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="V42" s="24">
         <f t="shared" si="23"/>
@@ -11040,13 +11133,13 @@
       </c>
       <c r="W42" s="24">
         <f t="shared" si="23"/>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B43" s="24">
         <f>B14</f>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C43" s="24">
         <f t="shared" ref="C43:I43" si="24">C14</f>
@@ -11054,7 +11147,7 @@
       </c>
       <c r="D43" s="24">
         <f t="shared" si="24"/>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E43" s="24">
         <f t="shared" si="24"/>
@@ -11062,7 +11155,7 @@
       </c>
       <c r="F43" s="24">
         <f t="shared" si="24"/>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="G43" s="24">
         <f t="shared" si="24"/>
@@ -11082,7 +11175,7 @@
       </c>
       <c r="P43" s="24">
         <f>P14</f>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Q43" s="24">
         <f t="shared" ref="Q43:W43" si="25">Q14</f>
@@ -11094,7 +11187,7 @@
       </c>
       <c r="S43" s="24">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="T43" s="24">
         <f t="shared" si="25"/>
@@ -11106,7 +11199,7 @@
       </c>
       <c r="V43" s="24">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="W43" s="24">
         <f t="shared" si="25"/>
@@ -11314,7 +11407,7 @@
     <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B48">
         <f>SUM(B42:B46)*$K$43</f>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <f t="shared" ref="C48:I48" si="32">SUM(C42:C46)*$K$43</f>
@@ -11322,7 +11415,7 @@
       </c>
       <c r="D48">
         <f t="shared" si="32"/>
-        <v>36375</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <f t="shared" si="32"/>
@@ -11330,11 +11423,11 @@
       </c>
       <c r="F48">
         <f t="shared" si="32"/>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <f t="shared" si="32"/>
-        <v>22625</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <f t="shared" si="32"/>
@@ -11361,53 +11454,68 @@
     <mergeCell ref="O5:W5"/>
     <mergeCell ref="A17:I17"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:I10">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="B10:I10 K10">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:I16">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:I22">
-    <cfRule type="cellIs" dxfId="7" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:I28">
-    <cfRule type="cellIs" dxfId="6" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:I34">
-    <cfRule type="cellIs" dxfId="5" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10:W10">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:W16">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22:W22">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:W28">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:W34">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y10">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11421,7 +11529,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection sqref="A1:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11500,7 +11608,7 @@
       </c>
       <c r="C4" s="28">
         <f>Inventario_Dinamico!B38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="D4" s="28">
         <f>Inventario_Dinamico!C38</f>
@@ -11508,7 +11616,7 @@
       </c>
       <c r="E4" s="28">
         <f>Inventario_Dinamico!D38</f>
-        <v>4600</v>
+        <v>0</v>
       </c>
       <c r="F4" s="28">
         <f>Inventario_Dinamico!E38</f>
@@ -11516,11 +11624,11 @@
       </c>
       <c r="G4" s="28">
         <f>Inventario_Dinamico!F38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H4" s="28">
         <f>Inventario_Dinamico!G38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="I4" s="28">
         <f>Inventario_Dinamico!H38</f>
@@ -11537,7 +11645,7 @@
       </c>
       <c r="C5" s="43">
         <f>Inventario_Dinamico!P38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="D5" s="43">
         <f>Inventario_Dinamico!Q38</f>
@@ -11545,11 +11653,11 @@
       </c>
       <c r="E5" s="43">
         <f>Inventario_Dinamico!R38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="43">
         <f>Inventario_Dinamico!S38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G5" s="43">
         <f>Inventario_Dinamico!T38</f>
@@ -11557,22 +11665,22 @@
       </c>
       <c r="H5" s="43">
         <f>Inventario_Dinamico!U38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="I5" s="43">
         <f>Inventario_Dinamico!V38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="J5" s="43">
         <f>Inventario_Dinamico!W38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="C6" s="28">
         <f t="shared" ref="C6:J6" si="0">SUM(C4:C5)</f>
-        <v>2300</v>
+        <v>6000</v>
       </c>
       <c r="D6" s="28">
         <f t="shared" si="0"/>
@@ -11580,27 +11688,27 @@
       </c>
       <c r="E6" s="28">
         <f t="shared" si="0"/>
-        <v>10600</v>
+        <v>0</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G6" s="28">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H6" s="28">
         <f t="shared" si="0"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="I6" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="J6" s="28">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -11621,35 +11729,35 @@
       </c>
       <c r="C8" s="28">
         <f>Inventario_Dinamico!B37</f>
-        <v>2367</v>
+        <v>9416.4</v>
       </c>
       <c r="D8" s="28">
         <f>Inventario_Dinamico!C37</f>
-        <v>1566</v>
+        <v>8508</v>
       </c>
       <c r="E8" s="28">
         <f>Inventario_Dinamico!D37</f>
-        <v>3384</v>
+        <v>7599.5999999999995</v>
       </c>
       <c r="F8" s="28">
         <f>Inventario_Dinamico!E37</f>
-        <v>2583</v>
+        <v>6691.2</v>
       </c>
       <c r="G8" s="28">
         <f>Inventario_Dinamico!F37</f>
-        <v>2772</v>
+        <v>5782.8</v>
       </c>
       <c r="H8" s="28">
         <f>Inventario_Dinamico!G37</f>
-        <v>3600</v>
+        <v>4874.3999999999996</v>
       </c>
       <c r="I8" s="28">
         <f>Inventario_Dinamico!H37</f>
-        <v>2799</v>
+        <v>3966</v>
       </c>
       <c r="J8" s="28">
         <f>Inventario_Dinamico!I37</f>
-        <v>1998</v>
+        <v>3057.6</v>
       </c>
       <c r="K8" t="str">
         <f>+VLOOKUP(Inputs!B110,Inputs!A107:C109,3,FALSE)</f>
@@ -11662,35 +11770,35 @@
       </c>
       <c r="C9" s="43">
         <f>Inventario_Dinamico!P37</f>
-        <v>601.5</v>
+        <v>5858.94</v>
       </c>
       <c r="D9" s="43">
         <f>Inventario_Dinamico!Q37</f>
-        <v>421.5</v>
+        <v>5677.3799999999992</v>
       </c>
       <c r="E9" s="43">
         <f>Inventario_Dinamico!R37</f>
-        <v>565.5</v>
+        <v>5495.8199999999988</v>
       </c>
       <c r="F9" s="43">
         <f>Inventario_Dinamico!S37</f>
-        <v>385.5</v>
+        <v>5555.4599999999991</v>
       </c>
       <c r="G9" s="43">
         <f>Inventario_Dinamico!T37</f>
-        <v>205.5</v>
+        <v>5373.9</v>
       </c>
       <c r="H9" s="43">
         <f>Inventario_Dinamico!U37</f>
-        <v>349.5</v>
+        <v>5192.3399999999992</v>
       </c>
       <c r="I9" s="43">
         <f>Inventario_Dinamico!V37</f>
-        <v>169.5</v>
+        <v>5251.98</v>
       </c>
       <c r="J9" s="43">
         <f>Inventario_Dinamico!W37</f>
-        <v>313.5</v>
+        <v>5070.4199999999992</v>
       </c>
       <c r="K9" t="str">
         <f>VLOOKUP(Inputs!B118,Inputs!A114:C117,3,FALSE)</f>
@@ -11700,35 +11808,35 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" s="28">
         <f t="shared" ref="C10:J10" si="1">+SUM(C8:C9)</f>
-        <v>2968.5</v>
+        <v>15275.34</v>
       </c>
       <c r="D10" s="28">
         <f t="shared" si="1"/>
-        <v>1987.5</v>
+        <v>14185.38</v>
       </c>
       <c r="E10" s="28">
         <f t="shared" si="1"/>
-        <v>3949.5</v>
+        <v>13095.419999999998</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" si="1"/>
-        <v>2968.5</v>
+        <v>12246.66</v>
       </c>
       <c r="G10" s="28">
         <f t="shared" si="1"/>
-        <v>2977.5</v>
+        <v>11156.7</v>
       </c>
       <c r="H10" s="28">
         <f t="shared" si="1"/>
-        <v>3949.5</v>
+        <v>10066.739999999998</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" si="1"/>
-        <v>2968.5</v>
+        <v>9217.98</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" si="1"/>
-        <v>2311.5</v>
+        <v>8128.0199999999986</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -11745,7 +11853,7 @@
       </c>
       <c r="C12" s="1">
         <f>(Inventario_Dinamico!B8+Inventario_Dinamico!B14+Inventario_Dinamico!B20+Inventario_Dinamico!B26+Inventario_Dinamico!B32)*$L$12</f>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <f>(Inventario_Dinamico!C8+Inventario_Dinamico!C14+Inventario_Dinamico!C20+Inventario_Dinamico!C26+Inventario_Dinamico!C32)*$L$12</f>
@@ -11753,7 +11861,7 @@
       </c>
       <c r="E12" s="1">
         <f>(Inventario_Dinamico!D8+Inventario_Dinamico!D14+Inventario_Dinamico!D20+Inventario_Dinamico!D26+Inventario_Dinamico!D32)*$L$12</f>
-        <v>36375</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <f>(Inventario_Dinamico!E8+Inventario_Dinamico!E14+Inventario_Dinamico!E20+Inventario_Dinamico!E26+Inventario_Dinamico!E32)*$L$12</f>
@@ -11761,11 +11869,11 @@
       </c>
       <c r="G12" s="1">
         <f>(Inventario_Dinamico!F8+Inventario_Dinamico!F14+Inventario_Dinamico!F20+Inventario_Dinamico!F26+Inventario_Dinamico!F32)*$L$12</f>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
         <f>(Inventario_Dinamico!G8+Inventario_Dinamico!G14+Inventario_Dinamico!G20+Inventario_Dinamico!G26+Inventario_Dinamico!G32)*$L$12</f>
-        <v>22625</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
         <f>(Inventario_Dinamico!H8+Inventario_Dinamico!H14+Inventario_Dinamico!H20+Inventario_Dinamico!H26+Inventario_Dinamico!H32)*$L$12</f>
@@ -11786,7 +11894,7 @@
       </c>
       <c r="C13" s="1">
         <f>(Inventario_Dinamico!P8+Inventario_Dinamico!P14+Inventario_Dinamico!P20+Inventario_Dinamico!P26+Inventario_Dinamico!P32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="D13" s="1">
         <f>(Inventario_Dinamico!Q8+Inventario_Dinamico!Q14+Inventario_Dinamico!Q20+Inventario_Dinamico!Q26+Inventario_Dinamico!Q32)*$L$13</f>
@@ -11794,11 +11902,11 @@
       </c>
       <c r="E13" s="1">
         <f>(Inventario_Dinamico!R8+Inventario_Dinamico!R14+Inventario_Dinamico!R20+Inventario_Dinamico!R26+Inventario_Dinamico!R32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <f>(Inventario_Dinamico!S8+Inventario_Dinamico!S14+Inventario_Dinamico!S20+Inventario_Dinamico!S26+Inventario_Dinamico!S32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="G13" s="1">
         <f>(Inventario_Dinamico!T8+Inventario_Dinamico!T14+Inventario_Dinamico!T20+Inventario_Dinamico!T26+Inventario_Dinamico!T32)*$L$13</f>
@@ -11806,15 +11914,15 @@
       </c>
       <c r="H13" s="1">
         <f>(Inventario_Dinamico!U8+Inventario_Dinamico!U14+Inventario_Dinamico!U20+Inventario_Dinamico!U26+Inventario_Dinamico!U32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <f>(Inventario_Dinamico!V8+Inventario_Dinamico!V14+Inventario_Dinamico!V20+Inventario_Dinamico!V26+Inventario_Dinamico!V32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="J13" s="1">
         <f>(Inventario_Dinamico!W8+Inventario_Dinamico!W14+Inventario_Dinamico!W20+Inventario_Dinamico!W26+Inventario_Dinamico!W32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <f>+VLOOKUP(Inputs!B118,Inputs!A114:B117,2,FALSE)</f>
@@ -11827,7 +11935,7 @@
       </c>
       <c r="B14" s="28">
         <f>BOM_Consumo_Piezas!P6+BOM_Consumo_Piezas!P16+BOM_Consumo_Piezas!P26+BOM_Consumo_Piezas!P36+BOM_Consumo_Piezas!P46</f>
-        <v>11520</v>
+        <v>14580</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -11844,7 +11952,7 @@
       </c>
       <c r="B15" s="28">
         <f>BOM_Consumo_Piezas!P7+BOM_Consumo_Piezas!P17+BOM_Consumo_Piezas!P27+BOM_Consumo_Piezas!P37+BOM_Consumo_Piezas!P47</f>
-        <v>12677</v>
+        <v>13391</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -11861,7 +11969,7 @@
       </c>
       <c r="B16" s="28">
         <f>BOM_Consumo_Piezas!P8+BOM_Consumo_Piezas!P18+BOM_Consumo_Piezas!P28+BOM_Consumo_Piezas!P38+BOM_Consumo_Piezas!P48</f>
-        <v>7776</v>
+        <v>8712</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -11878,7 +11986,7 @@
       </c>
       <c r="B17" s="28">
         <f>BOM_Consumo_Piezas!P9+BOM_Consumo_Piezas!P19+BOM_Consumo_Piezas!P29+BOM_Consumo_Piezas!P39+BOM_Consumo_Piezas!P49</f>
-        <v>5256</v>
+        <v>5808</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -11895,7 +12003,7 @@
       </c>
       <c r="B18" s="28">
         <f>BOM_Consumo_Piezas!P10+BOM_Consumo_Piezas!P20+BOM_Consumo_Piezas!P30+BOM_Consumo_Piezas!P40+BOM_Consumo_Piezas!P50</f>
-        <v>13320</v>
+        <v>14520</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -11912,7 +12020,7 @@
       </c>
       <c r="B19" s="43">
         <f>BOM_Consumo_Piezas!P11+BOM_Consumo_Piezas!P21+BOM_Consumo_Piezas!P31+BOM_Consumo_Piezas!P41+BOM_Consumo_Piezas!P51</f>
-        <v>3080</v>
+        <v>3388</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
@@ -11926,11 +12034,11 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <f>SUM(B12:B19)</f>
-        <v>53629</v>
+        <v>60399</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:J20" si="2">SUM(C12:C19)</f>
-        <v>13750</v>
+        <v>22110</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
@@ -11938,27 +12046,27 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>66075</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="2"/>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
-        <v>52325</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="2"/>
-        <v>29700</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12049,7 +12157,7 @@
       </c>
       <c r="C4" s="28">
         <f>Inventario_Dinamico!B38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="D4" s="28">
         <f>Inventario_Dinamico!C38</f>
@@ -12057,7 +12165,7 @@
       </c>
       <c r="E4" s="28">
         <f>Inventario_Dinamico!D38</f>
-        <v>4600</v>
+        <v>0</v>
       </c>
       <c r="F4" s="28">
         <f>Inventario_Dinamico!E38</f>
@@ -12065,11 +12173,11 @@
       </c>
       <c r="G4" s="28">
         <f>Inventario_Dinamico!F38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H4" s="28">
         <f>Inventario_Dinamico!G38</f>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="I4" s="28">
         <f>Inventario_Dinamico!H38</f>
@@ -12086,7 +12194,7 @@
       </c>
       <c r="C5" s="43">
         <f>Inventario_Dinamico!P38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="D5" s="43">
         <f>Inventario_Dinamico!Q38</f>
@@ -12094,11 +12202,11 @@
       </c>
       <c r="E5" s="43">
         <f>Inventario_Dinamico!R38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="43">
         <f>Inventario_Dinamico!S38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G5" s="43">
         <f>Inventario_Dinamico!T38</f>
@@ -12106,22 +12214,22 @@
       </c>
       <c r="H5" s="43">
         <f>Inventario_Dinamico!U38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="I5" s="43">
         <f>Inventario_Dinamico!V38</f>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="J5" s="43">
         <f>Inventario_Dinamico!W38</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="C6" s="28">
         <f t="shared" ref="C6:J6" si="0">SUM(C4:C5)</f>
-        <v>2300</v>
+        <v>6000</v>
       </c>
       <c r="D6" s="28">
         <f t="shared" si="0"/>
@@ -12129,27 +12237,27 @@
       </c>
       <c r="E6" s="28">
         <f t="shared" si="0"/>
-        <v>10600</v>
+        <v>0</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G6" s="28">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H6" s="28">
         <f t="shared" si="0"/>
-        <v>8300</v>
+        <v>0</v>
       </c>
       <c r="I6" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="J6" s="28">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -12170,35 +12278,35 @@
       </c>
       <c r="C8" s="28">
         <f>Inventario_Dinamico!B37</f>
-        <v>2367</v>
+        <v>9416.4</v>
       </c>
       <c r="D8" s="28">
         <f>Inventario_Dinamico!C37</f>
-        <v>1566</v>
+        <v>8508</v>
       </c>
       <c r="E8" s="28">
         <f>Inventario_Dinamico!D37</f>
-        <v>3384</v>
+        <v>7599.5999999999995</v>
       </c>
       <c r="F8" s="28">
         <f>Inventario_Dinamico!E37</f>
-        <v>2583</v>
+        <v>6691.2</v>
       </c>
       <c r="G8" s="28">
         <f>Inventario_Dinamico!F37</f>
-        <v>2772</v>
+        <v>5782.8</v>
       </c>
       <c r="H8" s="28">
         <f>Inventario_Dinamico!G37</f>
-        <v>3600</v>
+        <v>4874.3999999999996</v>
       </c>
       <c r="I8" s="28">
         <f>Inventario_Dinamico!H37</f>
-        <v>2799</v>
+        <v>3966</v>
       </c>
       <c r="J8" s="28">
         <f>Inventario_Dinamico!I37</f>
-        <v>1998</v>
+        <v>3057.6</v>
       </c>
       <c r="K8" t="str">
         <f>+VLOOKUP(Inputs!B110,Inputs!A107:C109,3,FALSE)</f>
@@ -12211,35 +12319,35 @@
       </c>
       <c r="C9" s="43">
         <f>Inventario_Dinamico!P37</f>
-        <v>601.5</v>
+        <v>5858.94</v>
       </c>
       <c r="D9" s="43">
         <f>Inventario_Dinamico!Q37</f>
-        <v>421.5</v>
+        <v>5677.3799999999992</v>
       </c>
       <c r="E9" s="43">
         <f>Inventario_Dinamico!R37</f>
-        <v>565.5</v>
+        <v>5495.8199999999988</v>
       </c>
       <c r="F9" s="43">
         <f>Inventario_Dinamico!S37</f>
-        <v>385.5</v>
+        <v>5555.4599999999991</v>
       </c>
       <c r="G9" s="43">
         <f>Inventario_Dinamico!T37</f>
-        <v>205.5</v>
+        <v>5373.9</v>
       </c>
       <c r="H9" s="43">
         <f>Inventario_Dinamico!U37</f>
-        <v>349.5</v>
+        <v>5192.3399999999992</v>
       </c>
       <c r="I9" s="43">
         <f>Inventario_Dinamico!V37</f>
-        <v>169.5</v>
+        <v>5251.98</v>
       </c>
       <c r="J9" s="43">
         <f>Inventario_Dinamico!W37</f>
-        <v>313.5</v>
+        <v>5070.4199999999992</v>
       </c>
       <c r="K9" t="str">
         <f>VLOOKUP(Inputs!B118,Inputs!A114:C117,3,FALSE)</f>
@@ -12249,35 +12357,35 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="28">
         <f t="shared" ref="C10:J10" si="1">+SUM(C8:C9)</f>
-        <v>2968.5</v>
+        <v>15275.34</v>
       </c>
       <c r="D10" s="28">
         <f t="shared" si="1"/>
-        <v>1987.5</v>
+        <v>14185.38</v>
       </c>
       <c r="E10" s="28">
         <f t="shared" si="1"/>
-        <v>3949.5</v>
+        <v>13095.419999999998</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" si="1"/>
-        <v>2968.5</v>
+        <v>12246.66</v>
       </c>
       <c r="G10" s="28">
         <f t="shared" si="1"/>
-        <v>2977.5</v>
+        <v>11156.7</v>
       </c>
       <c r="H10" s="28">
         <f t="shared" si="1"/>
-        <v>3949.5</v>
+        <v>10066.739999999998</v>
       </c>
       <c r="I10" s="28">
         <f t="shared" si="1"/>
-        <v>2968.5</v>
+        <v>9217.98</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" si="1"/>
-        <v>2311.5</v>
+        <v>8128.0199999999986</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -12291,7 +12399,7 @@
       </c>
       <c r="C12" s="1">
         <f>(Inventario_Dinamico!B8+Inventario_Dinamico!B14+Inventario_Dinamico!B20+Inventario_Dinamico!B26+Inventario_Dinamico!B32)*$L$12</f>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <f>(Inventario_Dinamico!C8+Inventario_Dinamico!C14+Inventario_Dinamico!C20+Inventario_Dinamico!C26+Inventario_Dinamico!C32)*$L$12</f>
@@ -12299,7 +12407,7 @@
       </c>
       <c r="E12" s="1">
         <f>(Inventario_Dinamico!D8+Inventario_Dinamico!D14+Inventario_Dinamico!D20+Inventario_Dinamico!D26+Inventario_Dinamico!D32)*$L$12</f>
-        <v>36375</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <f>(Inventario_Dinamico!E8+Inventario_Dinamico!E14+Inventario_Dinamico!E20+Inventario_Dinamico!E26+Inventario_Dinamico!E32)*$L$12</f>
@@ -12307,11 +12415,11 @@
       </c>
       <c r="G12" s="1">
         <f>(Inventario_Dinamico!F8+Inventario_Dinamico!F14+Inventario_Dinamico!F20+Inventario_Dinamico!F26+Inventario_Dinamico!F32)*$L$12</f>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
         <f>(Inventario_Dinamico!G8+Inventario_Dinamico!G14+Inventario_Dinamico!G20+Inventario_Dinamico!G26+Inventario_Dinamico!G32)*$L$12</f>
-        <v>22625</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
         <f>(Inventario_Dinamico!H8+Inventario_Dinamico!H14+Inventario_Dinamico!H20+Inventario_Dinamico!H26+Inventario_Dinamico!H32)*$L$12</f>
@@ -12332,7 +12440,7 @@
       </c>
       <c r="C13" s="1">
         <f>(Inventario_Dinamico!P8+Inventario_Dinamico!P14+Inventario_Dinamico!P20+Inventario_Dinamico!P26+Inventario_Dinamico!P32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="D13" s="1">
         <f>(Inventario_Dinamico!Q8+Inventario_Dinamico!Q14+Inventario_Dinamico!Q20+Inventario_Dinamico!Q26+Inventario_Dinamico!Q32)*$L$13</f>
@@ -12340,11 +12448,11 @@
       </c>
       <c r="E13" s="1">
         <f>(Inventario_Dinamico!R8+Inventario_Dinamico!R14+Inventario_Dinamico!R20+Inventario_Dinamico!R26+Inventario_Dinamico!R32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <f>(Inventario_Dinamico!S8+Inventario_Dinamico!S14+Inventario_Dinamico!S20+Inventario_Dinamico!S26+Inventario_Dinamico!S32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="G13" s="1">
         <f>(Inventario_Dinamico!T8+Inventario_Dinamico!T14+Inventario_Dinamico!T20+Inventario_Dinamico!T26+Inventario_Dinamico!T32)*$L$13</f>
@@ -12352,15 +12460,15 @@
       </c>
       <c r="H13" s="1">
         <f>(Inventario_Dinamico!U8+Inventario_Dinamico!U14+Inventario_Dinamico!U20+Inventario_Dinamico!U26+Inventario_Dinamico!U32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
         <f>(Inventario_Dinamico!V8+Inventario_Dinamico!V14+Inventario_Dinamico!V20+Inventario_Dinamico!V26+Inventario_Dinamico!V32)*$L$13</f>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="J13" s="1">
         <f>(Inventario_Dinamico!W8+Inventario_Dinamico!W14+Inventario_Dinamico!W20+Inventario_Dinamico!W26+Inventario_Dinamico!W32)*$L$13</f>
-        <v>29700</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <f>+VLOOKUP(Inputs!B118,Inputs!A114:B117,2,FALSE)</f>
@@ -12373,7 +12481,7 @@
       </c>
       <c r="B14" s="28">
         <f>BOM_Consumo_Piezas!P6+BOM_Consumo_Piezas!P16+BOM_Consumo_Piezas!P26+BOM_Consumo_Piezas!P36+BOM_Consumo_Piezas!P46</f>
-        <v>11520</v>
+        <v>14580</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -12390,7 +12498,7 @@
       </c>
       <c r="B15" s="28">
         <f>BOM_Consumo_Piezas!P7+BOM_Consumo_Piezas!P17+BOM_Consumo_Piezas!P27+BOM_Consumo_Piezas!P37+BOM_Consumo_Piezas!P47</f>
-        <v>12677</v>
+        <v>13391</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -12407,7 +12515,7 @@
       </c>
       <c r="B16" s="28">
         <f>BOM_Consumo_Piezas!P8+BOM_Consumo_Piezas!P18+BOM_Consumo_Piezas!P28+BOM_Consumo_Piezas!P38+BOM_Consumo_Piezas!P48</f>
-        <v>7776</v>
+        <v>8712</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -12424,7 +12532,7 @@
       </c>
       <c r="B17" s="28">
         <f>BOM_Consumo_Piezas!P9+BOM_Consumo_Piezas!P19+BOM_Consumo_Piezas!P29+BOM_Consumo_Piezas!P39+BOM_Consumo_Piezas!P49</f>
-        <v>5256</v>
+        <v>5808</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -12441,7 +12549,7 @@
       </c>
       <c r="B18" s="28">
         <f>BOM_Consumo_Piezas!P10+BOM_Consumo_Piezas!P20+BOM_Consumo_Piezas!P30+BOM_Consumo_Piezas!P40+BOM_Consumo_Piezas!P50</f>
-        <v>13320</v>
+        <v>14520</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -12458,7 +12566,7 @@
       </c>
       <c r="B19" s="43">
         <f>BOM_Consumo_Piezas!P11+BOM_Consumo_Piezas!P21+BOM_Consumo_Piezas!P31+BOM_Consumo_Piezas!P41+BOM_Consumo_Piezas!P51</f>
-        <v>3080</v>
+        <v>3388</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
@@ -12472,11 +12580,11 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <f>SUM(B12:B19)</f>
-        <v>53629</v>
+        <v>60399</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:J20" si="2">SUM(C12:C19)</f>
-        <v>13750</v>
+        <v>22110</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
@@ -12484,27 +12592,27 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>66075</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="2"/>
-        <v>13750</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
-        <v>52325</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22110</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="2"/>
-        <v>29700</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>